<commit_message>
Interfaz, restaurante y agregar
</commit_message>
<xml_diff>
--- a/Files/Compradores.xlsx
+++ b/Files/Compradores.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Lab2EDD\Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -16,6 +21,53 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>RutaArchivo</t>
+  </si>
+  <si>
+    <t>Files/ElSaborAlejandro.xlsx</t>
+  </si>
+  <si>
+    <t>Files/ElSaborAlexander.xlsx</t>
+  </si>
+  <si>
+    <t>Files/ElSaborAna.xlsx</t>
+  </si>
+  <si>
+    <t>Files/ElSaborJose.xlsx</t>
+  </si>
+  <si>
+    <t>Files/ElSaborJudith.xlsx</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Judith</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49,13 +101,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -68,8 +127,21 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla2" displayName="Tabla2" ref="A1:D6" totalsRowShown="0">
+  <autoFilter ref="A1:D6"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Usuario"/>
+    <tableColumn id="2" name="Contraseña"/>
+    <tableColumn id="3" name="Nombre"/>
+    <tableColumn id="4" name="RutaArchivo" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +186,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +221,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +403,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>